<commit_message>
added Execution steps for some ACS-ARE test cases
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/03_ACS-ARE-interaction/Test_cases_ACS_ARE.xlsx
+++ b/Tests/integrationTests/03_ACS-ARE-interaction/Test_cases_ACS_ARE.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
   <si>
     <t>Number</t>
   </si>
@@ -409,11 +409,6 @@
   <si>
     <t>ARE start file: start.bat (start.sh)
 ACS: ACS.exe
-activate model: CameraMouse.acs</t>
-  </si>
-  <si>
-    <t>ARE start file: start.bat (start.sh)
-ACS: ACS.exe
 model: demomenu.acs</t>
   </si>
   <si>
@@ -448,6 +443,64 @@
 ARE Status: 'Pause' 
 3. After clicking 'Start Model' button, the model GUI  must be shown and functional as expected
 ARE Status: 'Running'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Execute ARE start file
+2. Start ACS
+3. Click on 'Connect to ARE' button
+4. Click on 'Activate a stored Model', select the model 'ImageDemo.acs' and click onto OK
+</t>
+  </si>
+  <si>
+    <t>4.The 'ImageDemo.acs' model must be deployed and started on the ARE without error message</t>
+  </si>
+  <si>
+    <t>6.After setting autorun model, the AR E must start with the ImageDemo.acs model</t>
+  </si>
+  <si>
+    <t>ACS_ARE_11
+ARE start file: start.bat (start.sh)
+ACS: ACS.exe</t>
+  </si>
+  <si>
+    <t>1. Execute ARE start file
+2. Start ACS
+3. Click on 'Connect to ARE' button
+4. Click on 'Set as autorunl'
+5. Stop ARE
+6. Execute ARE start file
+7. Restore original demomenu.acs as autorun model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Execute ARE start file
+2. Start ACS
+3. Click on 'Connect to ARE' button
+4. Click on 'Load model from storage', select the model 'demomenu.acs' and click onto OK
+</t>
+  </si>
+  <si>
+    <t>4. The 'demomenu.acs' model must be loaded into the ACS Deployment tab and visualized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Execute ARE start file
+2. Start ACS
+3. Click on 'Connect to ARE' button
+4. Click on 'Download model'
+5. Click on 'Store model on ARE' and save model as 'demomenu_new.acs'
+</t>
+  </si>
+  <si>
+    <t>5. The ARE/models directory must contain a model called 'demomenu_new.acs'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Execute ARE start file
+2. Start ACS
+3. Click on 'Connect to ARE' button
+4. Click on 'Delete a stored model' and select 'demomenu_new.acs'
+</t>
+  </si>
+  <si>
+    <t>4. The ARE/models directory must not contain a model called 'demomenu_new.acs'</t>
   </si>
 </sst>
 </file>
@@ -834,7 +887,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -844,14 +897,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.140625" customWidth="1"/>
-    <col min="2" max="3" width="63" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="77" customWidth="1"/>
     <col min="6" max="6" width="58.7109375" customWidth="1"/>
@@ -998,7 +1052,7 @@
         <v>44</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -1019,7 +1073,7 @@
         <v>45</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -1040,7 +1094,7 @@
         <v>46</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -1082,7 +1136,7 @@
         <v>49</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -1162,8 +1216,12 @@
       <c r="D18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1177,10 +1235,14 @@
         <v>66</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1194,10 +1256,14 @@
         <v>66</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1211,10 +1277,14 @@
         <v>66</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1228,10 +1298,14 @@
         <v>66</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>